<commit_message>
verify if is a correct file delete spaces in data from file
</commit_message>
<xml_diff>
--- a/download/metasender.xlsx
+++ b/download/metasender.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">address</t>
+    <t xml:space="preserve">address_to_send</t>
   </si>
   <si>
     <t xml:space="preserve">amount</t>
@@ -35,7 +35,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -57,6 +57,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,8 +107,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -130,10 +140,10 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.83"/>
@@ -145,8 +155,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.83"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -154,16 +164,16 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>